<commit_message>
juiste versie van de tijdsplanning
</commit_message>
<xml_diff>
--- a/planning/tijdsplanning.xlsx
+++ b/planning/tijdsplanning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Wie</t>
   </si>
@@ -62,12 +62,6 @@
     <t>iedereen</t>
   </si>
   <si>
-    <t>wireframes maken</t>
-  </si>
-  <si>
-    <t>mockups maken</t>
-  </si>
-  <si>
     <t>database leren</t>
   </si>
   <si>
@@ -78,6 +72,39 @@
   </si>
   <si>
     <t>Stan</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>mockup over</t>
+  </si>
+  <si>
+    <t>Wout</t>
+  </si>
+  <si>
+    <t>mockup auto's</t>
+  </si>
+  <si>
+    <t>mockup contact</t>
+  </si>
+  <si>
+    <t>mockup inloggen</t>
+  </si>
+  <si>
+    <t>mockup registreren</t>
+  </si>
+  <si>
+    <t>wireframe inloggen</t>
+  </si>
+  <si>
+    <t>wireframe contact</t>
+  </si>
+  <si>
+    <t>wireframe over</t>
+  </si>
+  <si>
+    <t>wireframe home</t>
   </si>
 </sst>
 </file>
@@ -101,12 +128,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -216,15 +255,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -233,11 +268,199 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="27">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -524,13 +747,13 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
@@ -541,14 +764,14 @@
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="12">
+      <c r="B1" s="8">
         <f xml:space="preserve"> SUM(C4:C1048576)</f>
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="13">
+      <c r="E1" s="9">
         <f>MAX(D4:D1048576)</f>
         <v>42724</v>
       </c>
@@ -571,365 +794,389 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="15">
         <v>42724</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="14" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B15" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="8"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="8"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="8"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="8"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="8"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="8"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="8"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="8"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="8"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="8"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="8"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="8"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="8"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="8"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="8"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="8"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="8"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="8"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="8"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="8"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="8"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="8"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="8"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="8"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="8"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="8"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="4"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="8"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="8"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="4"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="8"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="4"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="8"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="4"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="8"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="4"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="8"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="4"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="8"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="4"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="8"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="4"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="10"/>
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="6"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
@@ -939,9 +1186,49 @@
       <c r="E51" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A4:E50">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$E4 &gt;0</formula>
+  <conditionalFormatting sqref="A22:E50 C5:E21">
+    <cfRule type="expression" dxfId="26" priority="2">
+      <formula>$E5 &gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="expression" dxfId="25" priority="4">
+      <formula>$E8 &gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16:B16">
+    <cfRule type="expression" dxfId="24" priority="6">
+      <formula>$E9 &gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="expression" dxfId="23" priority="8">
+      <formula>$E8 &gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:B15">
+    <cfRule type="expression" dxfId="22" priority="10">
+      <formula>$E7 &gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:B14">
+    <cfRule type="expression" dxfId="21" priority="12">
+      <formula>$E11 &gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:B7 A9:B9">
+    <cfRule type="expression" dxfId="20" priority="1">
+      <formula>$E1048575 &gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:B5">
+    <cfRule type="expression" dxfId="19" priority="14">
+      <formula>$E6 &gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:B13">
+    <cfRule type="expression" dxfId="18" priority="16">
+      <formula>$E7 &gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>